<commit_message>
Added the updated version of Supplemental Table 2.
</commit_message>
<xml_diff>
--- a/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_2.xlsx
+++ b/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Files\GCMP_TIR\immunity_microbiome\Supplemental_Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B71E2E-A934-4BE1-84C0-445CBACD58FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD6ADCD-1B69-4BD0-8D46-53C9A338A4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{DB1EA2F7-56E0-4613-8E16-F6B7EE6590B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB1EA2F7-56E0-4613-8E16-F6B7EE6590B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S2" sheetId="1" r:id="rId1"/>
@@ -74,16 +74,16 @@
     <t>TIR</t>
   </si>
   <si>
-    <t>Distribution of unique TIR, LRR, and Ig isoforms across sequenced coral genomes.</t>
-  </si>
-  <si>
     <t>LRR</t>
   </si>
   <si>
     <t>Ig</t>
   </si>
   <si>
-    <t>Table S2</t>
+    <t>Table S2: Distribution of unique TIR, LRR, and IG domain isoforms across sequenced coral genomes</t>
+  </si>
+  <si>
+    <t>Unique isofom copies of TIR, LRR, and Ig domains as annotated using Transdecoder to predict open reading frames followed by HMMER searched for the domains in the prediced reading frames.</t>
   </si>
 </sst>
 </file>
@@ -159,14 +159,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +484,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -493,187 +493,187 @@
     <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3">
+        <v>426</v>
+      </c>
+      <c r="D4" s="3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3">
+        <v>528</v>
+      </c>
+      <c r="D5" s="3">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3">
+        <v>339</v>
+      </c>
+      <c r="D6" s="3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3">
+        <v>838</v>
+      </c>
+      <c r="D7" s="3">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="C8" s="3">
+        <v>287</v>
+      </c>
+      <c r="D8" s="3">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
         <v>16</v>
       </c>
-      <c r="C4" s="5">
-        <v>426</v>
-      </c>
-      <c r="D4" s="5">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5">
+      <c r="C9" s="3">
+        <v>549</v>
+      </c>
+      <c r="D9" s="3">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>373</v>
+      </c>
+      <c r="D10" s="3">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3">
+        <v>454</v>
+      </c>
+      <c r="D11" s="3">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
         <v>17</v>
       </c>
-      <c r="C5" s="5">
-        <v>528</v>
-      </c>
-      <c r="D5" s="5">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5">
-        <v>14</v>
-      </c>
-      <c r="C6" s="5">
-        <v>339</v>
-      </c>
-      <c r="D6" s="5">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5">
-        <v>838</v>
-      </c>
-      <c r="D7" s="5">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5">
-        <v>287</v>
-      </c>
-      <c r="D8" s="5">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5">
-        <v>549</v>
-      </c>
-      <c r="D9" s="5">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5">
-        <v>373</v>
-      </c>
-      <c r="D10" s="5">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5">
-        <v>454</v>
-      </c>
-      <c r="D11" s="5">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5">
-        <v>17</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>536</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>749</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>18</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>612</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>747</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>21</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>519</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>764</v>
       </c>
     </row>

</xml_diff>